<commit_message>
Add Enter Air ENT.WA to Airlines overview sheet
</commit_message>
<xml_diff>
--- a/$RYAAY.xlsx
+++ b/$RYAAY.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20398"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E11F44-4F18-4549-A2C7-2CCD812AA6B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E36DA3E-783A-453A-BD7F-81E30E73E77B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28215" windowHeight="10245" xr2:uid="{1D564C9D-D6D5-40B3-8DFF-AA98636751CE}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>$RYAAY</t>
   </si>
@@ -110,6 +110,21 @@
   </si>
   <si>
     <t>Link</t>
+  </si>
+  <si>
+    <t>Lauda</t>
+  </si>
+  <si>
+    <t>Buzz</t>
+  </si>
+  <si>
+    <t>Malta Air</t>
+  </si>
+  <si>
+    <t>Ryan Air UK</t>
+  </si>
+  <si>
+    <t>Ryan Air</t>
   </si>
 </sst>
 </file>
@@ -117,7 +132,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="#,##0.0"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -263,15 +278,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -281,51 +287,60 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -357,7 +372,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>81001</xdr:rowOff>
+      <xdr:rowOff>109576</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -389,6 +404,67 @@
         <a:xfrm>
           <a:off x="2133600" y="219075"/>
           <a:ext cx="1847850" cy="214351"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>543223</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5" descr="Aviation Partners and Specialists">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CB5B4CD-D7FE-4DFE-A423-21CB1968321A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="13677900" y="514350"/>
+          <a:ext cx="1495723" cy="1276350"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -707,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DF6C741-3D41-493C-AF4A-F17D7B886566}">
-  <dimension ref="B2:E35"/>
+  <dimension ref="B2:R35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:D19"/>
+      <selection activeCell="U27" sqref="U27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -718,213 +794,241 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E2"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="3" t="s">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="R4" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B5" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="8" t="s">
+      <c r="C5" s="21"/>
+      <c r="D5" s="22"/>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="6">
         <v>69.05</v>
       </c>
-      <c r="D6" s="27"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="8" t="s">
+      <c r="D6" s="16"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="14">
         <v>227.43</v>
       </c>
-      <c r="D7" s="27"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="8" t="s">
+      <c r="D7" s="16"/>
+      <c r="R7" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="14">
         <f>C6*C7</f>
         <v>15704.041499999999</v>
       </c>
-      <c r="D8" s="27"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="8" t="s">
+      <c r="D8" s="16"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="27"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="8" t="s">
+      <c r="C9" s="14"/>
+      <c r="D9" s="16"/>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="27"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="8" t="s">
+      <c r="C10" s="14"/>
+      <c r="D10" s="16"/>
+      <c r="R10" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="25">
+      <c r="C11" s="14">
         <f>C9-C10</f>
         <v>0</v>
       </c>
-      <c r="D11" s="27"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="10" t="s">
+      <c r="D11" s="16"/>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="26">
+      <c r="C12" s="15">
         <f>C8-C11</f>
         <v>15704.041499999999</v>
       </c>
-      <c r="D12" s="28"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="3" t="s">
+      <c r="D12" s="17"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="R13" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B15" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="6" t="s">
+      <c r="C15" s="21"/>
+      <c r="D15" s="22"/>
+      <c r="R15" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="19"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="26"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="19"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="26"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="19"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="26"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="22"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="24"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="5"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="22"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="15"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="8"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="15"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="8"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="15"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="8"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="16"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="9"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="5"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="22"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="D30" s="19"/>
+      <c r="D30" s="26"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C31" s="18">
+      <c r="C31" s="25">
         <v>1984</v>
       </c>
-      <c r="D31" s="19"/>
+      <c r="D31" s="26"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="18">
+      <c r="C32" s="25">
         <v>1997</v>
       </c>
-      <c r="D32" s="19"/>
+      <c r="D32" s="26"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B33" s="17"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="19"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="26"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="23"/>
-      <c r="D34" s="24"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="13"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="20" t="s">
+      <c r="B35" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="21" t="s">
+      <c r="C35" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D35" s="22"/>
+      <c r="D35" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="C35:D35"/>
@@ -932,16 +1036,6 @@
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C30:D30"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>

</xml_diff>